<commit_message>
Sprint Logs updated with meeting 3
</commit_message>
<xml_diff>
--- a/Documents/Sprint_1_Logs.xlsx
+++ b/Documents/Sprint_1_Logs.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\smfol\Desktop\CMSC355_Group_Project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0B3EBADB-EE2F-4E5F-A8BD-F8B00CF14592}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7DB9DA01-8170-4F73-9C84-0052FF40D076}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{7DF3351B-E003-4528-89FF-8DC820A2E6C0}"/>
+    <workbookView xWindow="-80" yWindow="0" windowWidth="10290" windowHeight="7360" xr2:uid="{7DF3351B-E003-4528-89FF-8DC820A2E6C0}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="193" uniqueCount="73">
   <si>
     <t>Question</t>
   </si>
@@ -202,13 +202,61 @@
   </si>
   <si>
     <t>Not having a standard set of icons or images to use throughout the pages to keep consistent</t>
+  </si>
+  <si>
+    <t>Successfully connected the application to Google firebase. Utilizing the following set up for the andrio studio project: Download android studio v3.3.1 for windows from chrome using API 20:Andriod 4.4W (kitkat wear) for project API using Nexus 5x API with Nougat 24 OS for emulated device. Completed basic design for security question update page. Completed back end for security question page however does not consider user account or database, will have to e updated for password verification and to actually update database</t>
+  </si>
+  <si>
+    <t>Try to connect the submission of a security question with Google firebase</t>
+  </si>
+  <si>
+    <t>Installing Android studio from certain rowsers has proven to be problematic. So far google chrome has been issue free.</t>
+  </si>
+  <si>
+    <t>Versions od IDE, project, and emulator sohuld be consistent while in the rapid prototyping phase.</t>
+  </si>
+  <si>
+    <t>Continued work on sprites for the game</t>
+  </si>
+  <si>
+    <t>Continue to work on sprite animations and button code for the game</t>
+  </si>
+  <si>
+    <t>Nothing is currently getting in the way of  my work</t>
+  </si>
+  <si>
+    <t>Continue learning how to utilize new animation techniques</t>
+  </si>
+  <si>
+    <t>No changes need to be made to the project currently</t>
+  </si>
+  <si>
+    <t>Chores for spring break</t>
+  </si>
+  <si>
+    <t>documentation is tricky to master</t>
+  </si>
+  <si>
+    <t>I created maze concept art for level 3</t>
+  </si>
+  <si>
+    <t>No significant progress</t>
+  </si>
+  <si>
+    <t>Hopefully have the right design down for the help and about pages</t>
+  </si>
+  <si>
+    <t>Travel and Time Difference</t>
+  </si>
+  <si>
+    <t xml:space="preserve">It's easier to get work done when you can communcate with your team </t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -219,6 +267,27 @@
     <font>
       <sz val="11"/>
       <color rgb="FF222222"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -244,7 +313,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -252,6 +321,15 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -570,8 +648,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D7CED5CD-73C7-48F2-87A1-36C83338A6C8}">
   <dimension ref="A1:L21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E13" sqref="E13"/>
+    <sheetView tabSelected="1" topLeftCell="B3" workbookViewId="0">
+      <selection activeCell="E20" sqref="E20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -626,7 +704,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="2" spans="1:12" ht="68.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:12" ht="166" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
@@ -639,7 +717,9 @@
       <c r="D2" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="E2" s="1"/>
+      <c r="E2" s="5" t="s">
+        <v>57</v>
+      </c>
       <c r="F2" s="1"/>
       <c r="G2" s="1"/>
       <c r="H2" s="1"/>
@@ -658,7 +738,9 @@
       <c r="D3" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="E3" s="1"/>
+      <c r="E3" s="1" t="s">
+        <v>68</v>
+      </c>
       <c r="F3" s="1"/>
       <c r="G3" s="1"/>
       <c r="H3" s="1"/>
@@ -677,7 +759,9 @@
       <c r="D4" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="E4" s="1"/>
+      <c r="E4" s="1" t="s">
+        <v>69</v>
+      </c>
       <c r="F4" s="1"/>
       <c r="G4" s="1"/>
       <c r="H4" s="1"/>
@@ -696,7 +780,9 @@
       <c r="D5" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="E5" s="1"/>
+      <c r="E5" s="1" t="s">
+        <v>61</v>
+      </c>
       <c r="F5" s="1"/>
       <c r="G5" s="1"/>
       <c r="H5" s="1"/>
@@ -718,7 +804,9 @@
       <c r="D6" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="E6" s="1"/>
+      <c r="E6" s="1" t="s">
+        <v>58</v>
+      </c>
       <c r="F6" s="1"/>
       <c r="G6" s="1"/>
       <c r="H6" s="1"/>
@@ -737,7 +825,9 @@
       <c r="D7" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="E7" s="1"/>
+      <c r="E7" s="1" t="s">
+        <v>49</v>
+      </c>
       <c r="F7" s="1"/>
       <c r="G7" s="1"/>
       <c r="H7" s="1"/>
@@ -756,7 +846,9 @@
       <c r="D8" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="E8" s="1"/>
+      <c r="E8" s="1" t="s">
+        <v>70</v>
+      </c>
       <c r="F8" s="1"/>
       <c r="G8" s="1"/>
       <c r="H8" s="1"/>
@@ -775,7 +867,9 @@
       <c r="D9" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="E9" s="1"/>
+      <c r="E9" s="1" t="s">
+        <v>62</v>
+      </c>
       <c r="F9" s="1"/>
       <c r="G9" s="1"/>
       <c r="H9" s="1"/>
@@ -797,7 +891,9 @@
       <c r="D10" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="E10" s="1"/>
+      <c r="E10" s="1" t="s">
+        <v>25</v>
+      </c>
       <c r="F10" s="1"/>
       <c r="G10" s="1"/>
       <c r="H10" s="1"/>
@@ -816,7 +912,9 @@
       <c r="D11" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="E11" s="1"/>
+      <c r="E11" s="1" t="s">
+        <v>66</v>
+      </c>
       <c r="F11" s="1"/>
       <c r="G11" s="1"/>
       <c r="H11" s="1"/>
@@ -835,7 +933,9 @@
       <c r="D12" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="E12" s="1"/>
+      <c r="E12" s="1" t="s">
+        <v>71</v>
+      </c>
       <c r="F12" s="1"/>
       <c r="G12" s="1"/>
       <c r="H12" s="1"/>
@@ -854,7 +954,9 @@
       <c r="D13" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="E13" s="1"/>
+      <c r="E13" s="1" t="s">
+        <v>63</v>
+      </c>
       <c r="F13" s="1"/>
       <c r="G13" s="1"/>
       <c r="H13" s="1"/>
@@ -876,7 +978,9 @@
       <c r="D14" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="E14" s="1"/>
+      <c r="E14" s="6" t="s">
+        <v>59</v>
+      </c>
       <c r="F14" s="1"/>
       <c r="G14" s="1"/>
       <c r="H14" s="1"/>
@@ -895,7 +999,9 @@
       <c r="D15" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="E15" s="1"/>
+      <c r="E15" s="1" t="s">
+        <v>67</v>
+      </c>
       <c r="F15" s="1"/>
       <c r="G15" s="1"/>
       <c r="H15" s="1"/>
@@ -914,7 +1020,9 @@
       <c r="D16" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="E16" s="1"/>
+      <c r="E16" s="1" t="s">
+        <v>72</v>
+      </c>
       <c r="F16" s="1"/>
       <c r="G16" s="1"/>
       <c r="H16" s="1"/>
@@ -933,7 +1041,9 @@
       <c r="D17" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="E17" s="1"/>
+      <c r="E17" s="1" t="s">
+        <v>64</v>
+      </c>
       <c r="F17" s="1"/>
       <c r="G17" s="1"/>
       <c r="H17" s="1"/>
@@ -942,7 +1052,7 @@
       <c r="K17" s="1"/>
       <c r="L17" s="1"/>
     </row>
-    <row r="18" spans="1:12" ht="46" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:12" ht="61.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A18" s="1" t="s">
         <v>4</v>
       </c>
@@ -955,7 +1065,9 @@
       <c r="D18" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="E18" s="1"/>
+      <c r="E18" s="7" t="s">
+        <v>60</v>
+      </c>
       <c r="F18" s="1"/>
       <c r="G18" s="1"/>
       <c r="H18" s="1"/>
@@ -974,7 +1086,9 @@
       <c r="D19" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="E19" s="1"/>
+      <c r="E19" s="1" t="s">
+        <v>53</v>
+      </c>
       <c r="F19" s="1"/>
       <c r="G19" s="1"/>
       <c r="H19" s="1"/>
@@ -993,7 +1107,9 @@
       <c r="D20" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="E20" s="1"/>
+      <c r="E20" s="1" t="s">
+        <v>27</v>
+      </c>
       <c r="F20" s="1"/>
       <c r="G20" s="1"/>
       <c r="H20" s="1"/>
@@ -1012,7 +1128,9 @@
       <c r="D21" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="E21" s="1"/>
+      <c r="E21" s="1" t="s">
+        <v>65</v>
+      </c>
       <c r="F21" s="1"/>
       <c r="G21" s="1"/>
       <c r="H21" s="1"/>

</xml_diff>

<commit_message>
Sprint 1 Logs 4-5 Added
</commit_message>
<xml_diff>
--- a/Documents/Sprint_1_Logs.xlsx
+++ b/Documents/Sprint_1_Logs.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\smfol\Desktop\CMSC355_Group_Project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7DB9DA01-8170-4F73-9C84-0052FF40D076}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8B57D992-2CE0-4E9F-8EBA-C85FFFFF818C}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-80" yWindow="0" windowWidth="10290" windowHeight="7360" xr2:uid="{7DF3351B-E003-4528-89FF-8DC820A2E6C0}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="193" uniqueCount="73">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="137" uniqueCount="96">
   <si>
     <t>Question</t>
   </si>
@@ -57,9 +57,6 @@
     <t xml:space="preserve">Gavin </t>
   </si>
   <si>
-    <t>Joe</t>
-  </si>
-  <si>
     <t>Sinead</t>
   </si>
   <si>
@@ -250,6 +247,78 @@
   </si>
   <si>
     <t xml:space="preserve">It's easier to get work done when you can communcate with your team </t>
+  </si>
+  <si>
+    <t>I worked on the security issue where the user I signed out after 5 minuts of activity</t>
+  </si>
+  <si>
+    <t xml:space="preserve">I will work on my assigned issues. Specifically the same issue as before. </t>
+  </si>
+  <si>
+    <t>Errands for spring break</t>
+  </si>
+  <si>
+    <t>Consistency is hard</t>
+  </si>
+  <si>
+    <t>Continued sprite work and completed the layout for the login screen</t>
+  </si>
+  <si>
+    <t>Continue sprite work and start coding the login screen</t>
+  </si>
+  <si>
+    <t>Began to learn how to create a login screen</t>
+  </si>
+  <si>
+    <t>Completed basic design for forgot information page. Completed back end for forgot information page however does not consider user account or databse, will have to be updated for security question answer verification</t>
+  </si>
+  <si>
+    <t>Will spend time looking into firebase utiliaztion</t>
+  </si>
+  <si>
+    <t>Nothing new as of yet</t>
+  </si>
+  <si>
+    <t>London</t>
+  </si>
+  <si>
+    <t>Nothing new</t>
+  </si>
+  <si>
+    <t>I created maze concept for level 4</t>
+  </si>
+  <si>
+    <t>Work on my assignments</t>
+  </si>
+  <si>
+    <t>Further work on assignments</t>
+  </si>
+  <si>
+    <t>Errand for spring break</t>
+  </si>
+  <si>
+    <t>Documentation is tricky to master</t>
+  </si>
+  <si>
+    <t>Joseph</t>
+  </si>
+  <si>
+    <t>Not enough time to complete anything. Had other work.</t>
+  </si>
+  <si>
+    <t>Creating more forms in the user settings</t>
+  </si>
+  <si>
+    <t>Nothing since last meeting</t>
+  </si>
+  <si>
+    <t>Continued sprit work and started layout for login page</t>
+  </si>
+  <si>
+    <t>Continue sprite work and complete login page</t>
+  </si>
+  <si>
+    <t>Learned a little about creating more complex page layouts</t>
   </si>
 </sst>
 </file>
@@ -648,8 +717,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D7CED5CD-73C7-48F2-87A1-36C83338A6C8}">
   <dimension ref="A1:L21"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B3" workbookViewId="0">
-      <selection activeCell="E20" sqref="E20"/>
+    <sheetView tabSelected="1" topLeftCell="D19" workbookViewId="0">
+      <selection activeCell="F20" sqref="F20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -674,34 +743,34 @@
         <v>5</v>
       </c>
       <c r="C1" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="D1" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="E1" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="E1" s="3" t="s">
+      <c r="F1" t="s">
         <v>13</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>14</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>15</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="I1" s="3" t="s">
+      <c r="J1" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="J1" s="3" t="s">
+      <c r="K1" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="K1" s="3" t="s">
+      <c r="L1" s="3" t="s">
         <v>19</v>
-      </c>
-      <c r="L1" s="3" t="s">
-        <v>20</v>
       </c>
     </row>
     <row r="2" spans="1:12" ht="166" customHeight="1" x14ac:dyDescent="0.35">
@@ -712,16 +781,20 @@
         <v>7</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="E2" s="5" t="s">
-        <v>57</v>
-      </c>
-      <c r="F2" s="1"/>
-      <c r="G2" s="1"/>
+        <v>56</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>79</v>
+      </c>
       <c r="H2" s="1"/>
       <c r="I2" s="1"/>
       <c r="J2" s="1"/>
@@ -730,19 +803,23 @@
     </row>
     <row r="3" spans="1:12" ht="66.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B3" t="s">
-        <v>8</v>
+        <v>89</v>
       </c>
       <c r="C3" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="D3" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="D3" s="1" t="s">
-        <v>47</v>
-      </c>
       <c r="E3" s="1" t="s">
-        <v>68</v>
-      </c>
-      <c r="F3" s="1"/>
-      <c r="G3" s="1"/>
+        <v>67</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="G3" s="1" t="s">
+        <v>72</v>
+      </c>
       <c r="H3" s="1"/>
       <c r="I3" s="1"/>
       <c r="J3" s="1"/>
@@ -751,19 +828,23 @@
     </row>
     <row r="4" spans="1:12" ht="68.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B4" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>69</v>
-      </c>
-      <c r="F4" s="1"/>
-      <c r="G4" s="1"/>
+        <v>68</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="G4" s="1" t="s">
+        <v>68</v>
+      </c>
       <c r="H4" s="1"/>
       <c r="I4" s="1"/>
       <c r="J4" s="1"/>
@@ -772,19 +853,23 @@
     </row>
     <row r="5" spans="1:12" ht="60" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B5" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="F5" s="1"/>
-      <c r="G5" s="1"/>
+        <v>60</v>
+      </c>
+      <c r="F5" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="G5" s="1" t="s">
+        <v>76</v>
+      </c>
       <c r="H5" s="1"/>
       <c r="I5" s="1"/>
       <c r="J5" s="1"/>
@@ -799,16 +884,20 @@
         <v>7</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>58</v>
-      </c>
-      <c r="F6" s="1"/>
-      <c r="G6" s="1"/>
+        <v>57</v>
+      </c>
+      <c r="F6" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="G6" s="1" t="s">
+        <v>80</v>
+      </c>
       <c r="H6" s="1"/>
       <c r="I6" s="1"/>
       <c r="J6" s="1"/>
@@ -817,19 +906,23 @@
     </row>
     <row r="7" spans="1:12" ht="57.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B7" t="s">
-        <v>8</v>
+        <v>89</v>
       </c>
       <c r="C7" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="D7" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="D7" s="1" t="s">
-        <v>49</v>
-      </c>
       <c r="E7" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="F7" s="1"/>
-      <c r="G7" s="1"/>
+        <v>48</v>
+      </c>
+      <c r="F7" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="G7" s="1" t="s">
+        <v>73</v>
+      </c>
       <c r="H7" s="1"/>
       <c r="I7" s="1"/>
       <c r="J7" s="1"/>
@@ -838,19 +931,23 @@
     </row>
     <row r="8" spans="1:12" ht="65" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B8" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>70</v>
-      </c>
-      <c r="F8" s="1"/>
-      <c r="G8" s="1"/>
+        <v>69</v>
+      </c>
+      <c r="F8" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="G8" s="1" t="s">
+        <v>86</v>
+      </c>
       <c r="H8" s="1"/>
       <c r="I8" s="1"/>
       <c r="J8" s="1"/>
@@ -859,19 +956,23 @@
     </row>
     <row r="9" spans="1:12" ht="64.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B9" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="F9" s="1"/>
-      <c r="G9" s="1"/>
+        <v>61</v>
+      </c>
+      <c r="F9" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="G9" s="1" t="s">
+        <v>77</v>
+      </c>
       <c r="H9" s="1"/>
       <c r="I9" s="1"/>
       <c r="J9" s="1"/>
@@ -886,16 +987,20 @@
         <v>7</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="F10" s="1"/>
-      <c r="G10" s="1"/>
+        <v>24</v>
+      </c>
+      <c r="F10" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="G10" s="1" t="s">
+        <v>24</v>
+      </c>
       <c r="H10" s="1"/>
       <c r="I10" s="1"/>
       <c r="J10" s="1"/>
@@ -904,19 +1009,23 @@
     </row>
     <row r="11" spans="1:12" ht="58" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B11" t="s">
-        <v>8</v>
+        <v>89</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="F11" s="1"/>
-      <c r="G11" s="1"/>
+        <v>65</v>
+      </c>
+      <c r="F11" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="G11" s="1" t="s">
+        <v>74</v>
+      </c>
       <c r="H11" s="1"/>
       <c r="I11" s="1"/>
       <c r="J11" s="1"/>
@@ -925,19 +1034,23 @@
     </row>
     <row r="12" spans="1:12" ht="59.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B12" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>71</v>
-      </c>
-      <c r="F12" s="1"/>
-      <c r="G12" s="1"/>
+        <v>70</v>
+      </c>
+      <c r="F12" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="G12" s="1" t="s">
+        <v>82</v>
+      </c>
       <c r="H12" s="1"/>
       <c r="I12" s="1"/>
       <c r="J12" s="1"/>
@@ -946,19 +1059,23 @@
     </row>
     <row r="13" spans="1:12" ht="57.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B13" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>63</v>
-      </c>
-      <c r="F13" s="1"/>
-      <c r="G13" s="1"/>
+        <v>62</v>
+      </c>
+      <c r="F13" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="G13" s="1" t="s">
+        <v>32</v>
+      </c>
       <c r="H13" s="1"/>
       <c r="I13" s="1"/>
       <c r="J13" s="1"/>
@@ -973,16 +1090,20 @@
         <v>7</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="E14" s="6" t="s">
-        <v>59</v>
-      </c>
-      <c r="F14" s="1"/>
-      <c r="G14" s="1"/>
+        <v>58</v>
+      </c>
+      <c r="F14" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="G14" s="1" t="s">
+        <v>81</v>
+      </c>
       <c r="H14" s="1"/>
       <c r="I14" s="1"/>
       <c r="J14" s="1"/>
@@ -991,19 +1112,23 @@
     </row>
     <row r="15" spans="1:12" ht="60" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B15" t="s">
-        <v>8</v>
+        <v>89</v>
       </c>
       <c r="C15" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="D15" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="D15" s="1" t="s">
-        <v>52</v>
-      </c>
       <c r="E15" s="1" t="s">
-        <v>67</v>
-      </c>
-      <c r="F15" s="1"/>
-      <c r="G15" s="1"/>
+        <v>66</v>
+      </c>
+      <c r="F15" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="G15" s="1" t="s">
+        <v>75</v>
+      </c>
       <c r="H15" s="1"/>
       <c r="I15" s="1"/>
       <c r="J15" s="1"/>
@@ -1012,19 +1137,23 @@
     </row>
     <row r="16" spans="1:12" ht="57.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B16" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="E16" s="1" t="s">
-        <v>72</v>
-      </c>
-      <c r="F16" s="1"/>
-      <c r="G16" s="1"/>
+        <v>71</v>
+      </c>
+      <c r="F16" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="G16" s="1" t="s">
+        <v>83</v>
+      </c>
       <c r="H16" s="1"/>
       <c r="I16" s="1"/>
       <c r="J16" s="1"/>
@@ -1033,19 +1162,23 @@
     </row>
     <row r="17" spans="1:12" ht="62" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B17" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="E17" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="F17" s="1"/>
-      <c r="G17" s="1"/>
+        <v>63</v>
+      </c>
+      <c r="F17" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="G17" s="1" t="s">
+        <v>78</v>
+      </c>
       <c r="H17" s="1"/>
       <c r="I17" s="1"/>
       <c r="J17" s="1"/>
@@ -1060,16 +1193,20 @@
         <v>7</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="E18" s="7" t="s">
-        <v>60</v>
-      </c>
-      <c r="F18" s="1"/>
-      <c r="G18" s="1"/>
+        <v>59</v>
+      </c>
+      <c r="F18" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="G18" s="1" t="s">
+        <v>24</v>
+      </c>
       <c r="H18" s="1"/>
       <c r="I18" s="1"/>
       <c r="J18" s="1"/>
@@ -1078,19 +1215,23 @@
     </row>
     <row r="19" spans="1:12" ht="59.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B19" t="s">
-        <v>8</v>
+        <v>89</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="E19" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="F19" s="1"/>
-      <c r="G19" s="1"/>
+        <v>52</v>
+      </c>
+      <c r="F19" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="G19" s="1" t="s">
+        <v>52</v>
+      </c>
       <c r="H19" s="1"/>
       <c r="I19" s="1"/>
       <c r="J19" s="1"/>
@@ -1099,19 +1240,23 @@
     </row>
     <row r="20" spans="1:12" ht="58" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B20" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="E20" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="F20" s="1"/>
-      <c r="G20" s="1"/>
+        <v>26</v>
+      </c>
+      <c r="F20" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="G20" s="1" t="s">
+        <v>26</v>
+      </c>
       <c r="H20" s="1"/>
       <c r="I20" s="1"/>
       <c r="J20" s="1"/>
@@ -1120,19 +1265,23 @@
     </row>
     <row r="21" spans="1:12" ht="60" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B21" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D21" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="E21" s="1" t="s">
-        <v>65</v>
-      </c>
-      <c r="F21" s="1"/>
-      <c r="G21" s="1"/>
+        <v>64</v>
+      </c>
+      <c r="F21" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="G21" s="1" t="s">
+        <v>64</v>
+      </c>
       <c r="H21" s="1"/>
       <c r="I21" s="1"/>
       <c r="J21" s="1"/>

</xml_diff>